<commit_message>
More documentation and comments
</commit_message>
<xml_diff>
--- a/results/GP_Ensemble_RMSE_split_comparison.xlsx
+++ b/results/GP_Ensemble_RMSE_split_comparison.xlsx
@@ -460,7 +460,7 @@
         <v>20</v>
       </c>
       <c r="C2" t="n">
-        <v>0.4438797652908861</v>
+        <v>0.5195787887265466</v>
       </c>
       <c r="D2" t="n">
         <v>0.4516313852738461</v>
@@ -476,7 +476,7 @@
         <v>20</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1748456441686702</v>
+        <v>0.1899731131478304</v>
       </c>
       <c r="D3" t="n">
         <v>0.2042034188482884</v>
@@ -540,7 +540,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.3833382349921633</v>
+        <v>0.308413692671376</v>
       </c>
       <c r="D8" t="n">
         <v>0.5430319550281784</v>
@@ -556,7 +556,7 @@
         <v>88</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1743028066319152</v>
+        <v>0.1734898436308585</v>
       </c>
       <c r="D9" t="n">
         <v>0.2410639273495594</v>
@@ -572,7 +572,7 @@
         <v>34</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1945659312824916</v>
+        <v>0.2055719433594982</v>
       </c>
       <c r="D10" t="n">
         <v>0.3046013568972082</v>

</xml_diff>